<commit_message>
Premier Commit Instrument Implementation
La deep-copie des classes Coupons et Rates sont faite.
</commit_message>
<xml_diff>
--- a/data/input/G_MatrixMapping_5YR.xlsx
+++ b/data/input/G_MatrixMapping_5YR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="18915" windowHeight="12330"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="18915" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Gmapping" sheetId="7" r:id="rId1"/>
@@ -19,9 +19,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="102">
-  <si>
-    <t>g_natrix</t>
-  </si>
   <si>
     <t>gTransformed</t>
   </si>
@@ -324,6 +321,9 @@
   </si>
   <si>
     <t xml:space="preserve">diff Interpolated-Init Matrix </t>
+  </si>
+  <si>
+    <t>g_matrix</t>
   </si>
 </sst>
 </file>
@@ -1413,23 +1413,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="119645696"/>
-        <c:axId val="119647232"/>
+        <c:axId val="141248000"/>
+        <c:axId val="141249536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119645696"/>
+        <c:axId val="141248000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119647232"/>
+        <c:crossAx val="141249536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119647232"/>
+        <c:axId val="141249536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1437,7 +1437,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119645696"/>
+        <c:crossAx val="141248000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1449,7 +1449,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1984,23 +1984,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="122776576"/>
-        <c:axId val="122782464"/>
+        <c:axId val="141650944"/>
+        <c:axId val="141652736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122776576"/>
+        <c:axId val="141650944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122782464"/>
+        <c:crossAx val="141652736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122782464"/>
+        <c:axId val="141652736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2008,7 +2008,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122776576"/>
+        <c:crossAx val="141650944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2020,7 +2020,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2675,23 +2675,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="122802560"/>
-        <c:axId val="122804096"/>
+        <c:axId val="141685120"/>
+        <c:axId val="141686656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122802560"/>
+        <c:axId val="141685120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122804096"/>
+        <c:crossAx val="141686656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122804096"/>
+        <c:axId val="141686656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2699,7 +2699,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122802560"/>
+        <c:crossAx val="141685120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2711,7 +2711,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3108,23 +3108,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="122848768"/>
-        <c:axId val="122850304"/>
+        <c:axId val="56858112"/>
+        <c:axId val="56859648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122848768"/>
+        <c:axId val="56858112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122850304"/>
+        <c:crossAx val="56859648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122850304"/>
+        <c:axId val="56859648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3132,7 +3132,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122848768"/>
+        <c:crossAx val="56858112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3144,7 +3144,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3541,23 +3541,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="122865920"/>
-        <c:axId val="122867712"/>
+        <c:axId val="56875264"/>
+        <c:axId val="62656512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122865920"/>
+        <c:axId val="56875264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122867712"/>
+        <c:crossAx val="62656512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122867712"/>
+        <c:axId val="62656512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3565,7 +3565,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122865920"/>
+        <c:crossAx val="56875264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3577,7 +3577,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3740,23 +3740,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="132406656"/>
-        <c:axId val="132428928"/>
+        <c:axId val="141528448"/>
+        <c:axId val="141546624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="132406656"/>
+        <c:axId val="141528448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132428928"/>
+        <c:crossAx val="141546624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132428928"/>
+        <c:axId val="141546624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3764,7 +3764,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132406656"/>
+        <c:crossAx val="141528448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3776,7 +3776,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3939,23 +3939,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="132334336"/>
-        <c:axId val="132335872"/>
+        <c:axId val="56980224"/>
+        <c:axId val="56981760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="132334336"/>
+        <c:axId val="56980224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132335872"/>
+        <c:crossAx val="56981760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132335872"/>
+        <c:axId val="56981760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3963,7 +3963,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132334336"/>
+        <c:crossAx val="56980224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3975,7 +3975,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4488,9 +4488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.7109375" defaultRowHeight="15"/>
   <cols>
@@ -4501,12 +4499,12 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
@@ -4544,7 +4542,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -4561,10 +4559,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>3</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>4</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -4580,13 +4578,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="12"/>
@@ -4601,16 +4599,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="E6" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="11"/>
@@ -4619,7 +4617,7 @@
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="M6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -4627,19 +4625,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="F7" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -4647,7 +4645,7 @@
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="M7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N7" s="6">
         <v>1</v>
@@ -4670,22 +4668,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="G8" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
@@ -4695,16 +4693,16 @@
         <v>1</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -4712,25 +4710,25 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="G9" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="H9" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
@@ -4739,13 +4737,13 @@
         <v>2</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -4753,28 +4751,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="G10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="I10" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
@@ -4782,10 +4780,10 @@
         <v>3</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -4793,38 +4791,38 @@
         <v>9</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="E11" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="F11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="G11" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="H11" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="I11" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="J11" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="K11" s="11"/>
       <c r="M11" s="6">
         <v>4</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -4832,34 +4830,34 @@
         <v>10</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="E12" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="F12" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="G12" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="H12" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="I12" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="J12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="K12" s="28" t="s">
         <v>55</v>
-      </c>
-      <c r="K12" s="28" t="s">
-        <v>56</v>
       </c>
       <c r="L12" s="11"/>
       <c r="M12" s="6">
@@ -4871,12 +4869,12 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="5">
         <v>1</v>
@@ -4909,7 +4907,7 @@
         <v>10</v>
       </c>
       <c r="M17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -4917,35 +4915,35 @@
         <v>1</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>3</v>
-      </c>
       <c r="D18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="H18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="I18" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="21" t="s">
+      <c r="J18" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="K18" s="11"/>
       <c r="M18" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N18" s="6">
         <v>1</v>
@@ -4968,44 +4966,44 @@
         <v>2</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J19" s="11"/>
       <c r="M19" s="6">
         <v>1</v>
       </c>
       <c r="N19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O19" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="O19" s="4" t="s">
+      <c r="P19" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P19" s="4" t="s">
+      <c r="Q19" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="Q19" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -5013,38 +5011,38 @@
         <v>3</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I20" s="11"/>
       <c r="M20" s="6">
         <v>2</v>
       </c>
       <c r="N20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="O20" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="O20" s="4" t="s">
+      <c r="P20" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="P20" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -5052,32 +5050,32 @@
         <v>4</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H21" s="11"/>
       <c r="M21" s="6">
         <v>3</v>
       </c>
       <c r="N21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O21" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -5085,26 +5083,26 @@
         <v>5</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G22" s="11"/>
       <c r="M22" s="6">
         <v>4</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -5112,16 +5110,16 @@
         <v>6</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F23" s="12"/>
       <c r="M23" s="6">
@@ -5133,13 +5131,13 @@
         <v>7</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="1"/>
@@ -5149,10 +5147,10 @@
         <v>8</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="11"/>
     </row>
@@ -5161,7 +5159,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="11"/>
       <c r="F26" s="1"/>
@@ -5329,16 +5327,16 @@
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="AF1" t="s">
         <v>60</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:37">
@@ -5427,22 +5425,22 @@
         <v>0</v>
       </c>
       <c r="AF2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AG2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AH2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AI2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AJ2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:37">
@@ -5531,22 +5529,22 @@
         <v>0</v>
       </c>
       <c r="AF3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK3" t="s">
         <v>62</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:37">
@@ -5635,22 +5633,22 @@
         <v>0</v>
       </c>
       <c r="AF4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>62</v>
       </c>
-      <c r="AG4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>63</v>
-      </c>
       <c r="AK4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:37">
@@ -5739,22 +5737,22 @@
         <v>0</v>
       </c>
       <c r="AF5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AI5" t="s">
         <v>62</v>
       </c>
-      <c r="AG5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>63</v>
-      </c>
       <c r="AJ5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AK5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -5843,22 +5841,22 @@
         <v>0</v>
       </c>
       <c r="AF6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH6" t="s">
         <v>62</v>
       </c>
-      <c r="AG6" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>63</v>
-      </c>
       <c r="AI6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AJ6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AK6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:37">
@@ -5947,22 +5945,22 @@
         <v>0</v>
       </c>
       <c r="AF7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG7" t="s">
         <v>62</v>
       </c>
-      <c r="AG7" t="s">
-        <v>63</v>
-      </c>
       <c r="AH7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AI7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AJ7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AK7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:37">
@@ -6325,37 +6323,37 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
         <v>84</v>
       </c>
-      <c r="B1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>86</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" t="s">
-        <v>88</v>
-      </c>
       <c r="N1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" t="s">
         <v>96</v>
-      </c>
-      <c r="O1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -8920,16 +8918,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
         <v>94</v>
-      </c>
-      <c r="C1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -9264,7 +9262,7 @@
   <sheetData>
     <row r="1" spans="1:30">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -12029,7 +12027,7 @@
     </row>
     <row r="34" spans="1:30">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:30">
@@ -14794,7 +14792,7 @@
     </row>
     <row r="67" spans="1:30">
       <c r="A67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:30">
@@ -17559,7 +17557,7 @@
     </row>
     <row r="100" spans="1:30">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:30">

</xml_diff>